<commit_message>
fix: add ban brand
</commit_message>
<xml_diff>
--- a/uploader/templates/ban/ban.xlsx
+++ b/uploader/templates/ban/ban.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gimsang-yun/asmama_crwaling/uploader/templates/ban/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C7A0DD-E947-B140-84E5-B0A0F3412B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6B5FFF-BF01-674E-8266-D0B0ACCB5678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="18000" xr2:uid="{E7FBD66D-C732-4E47-9A6D-32DB07996244}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="17380" xr2:uid="{E7FBD66D-C732-4E47-9A6D-32DB07996244}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3591" uniqueCount="1760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3592" uniqueCount="1761">
   <si>
     <t>주의 브랜드</t>
   </si>
@@ -5322,6 +5322,9 @@
   </si>
   <si>
     <t>닥터하스킨</t>
+  </si>
+  <si>
+    <t>달바</t>
   </si>
 </sst>
 </file>
@@ -6002,7 +6005,7 @@
   <dimension ref="A1:I1638"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1198" workbookViewId="0">
-      <selection activeCell="L1218" sqref="L1218"/>
+      <selection activeCell="D1221" sqref="D1221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -25738,7 +25741,9 @@
       <c r="I1217" s="1"/>
     </row>
     <row r="1218" spans="1:9">
-      <c r="A1218" s="1"/>
+      <c r="A1218" s="1" t="s">
+        <v>1760</v>
+      </c>
       <c r="B1218" s="1"/>
       <c r="C1218" s="1"/>
       <c r="D1218" s="1"/>

</xml_diff>